<commit_message>
move to airtable source/output
</commit_message>
<xml_diff>
--- a/gfm-campaign-details.xlsx
+++ b/gfm-campaign-details.xlsx
@@ -28,6 +28,114 @@
     <t>Error</t>
   </si>
   <si>
+    <t>The Casco Ohana affected by the Lahaina Fire</t>
+  </si>
+  <si>
+    <t>$59,060</t>
+  </si>
+  <si>
+    <t>$60,000</t>
+  </si>
+  <si>
+    <t>https://images.gofundme.com/-ni-okGZOFouWUbBuTswBKrJZok=/720x405/https://d2g8igdw686xgo.cloudfront.net/74641605_1691693515709506_r.jpeg</t>
+  </si>
+  <si>
+    <t>Timko Family Lahaina Wildfire Relief Fund</t>
+  </si>
+  <si>
+    <t>$12,540</t>
+  </si>
+  <si>
+    <t>$20,000</t>
+  </si>
+  <si>
+    <t>https://images.gofundme.com/c1UhbqWgLfq7yZCWg4xtWuIIGio=/720x405/https://d2g8igdw686xgo.cloudfront.net/74647267_1691705408863508_r.jpeg</t>
+  </si>
+  <si>
+    <t>Takafua Family Wildfire in Lahaina</t>
+  </si>
+  <si>
+    <t>$8,306</t>
+  </si>
+  <si>
+    <t>$100,000</t>
+  </si>
+  <si>
+    <t>https://images.gofundme.com/53DmfUFhgRdHzs8CJkFdtW0XNnY=/720x405/https://d2g8igdw686xgo.cloudfront.net/74675893_1692732096230158_r.jpg</t>
+  </si>
+  <si>
+    <t>Lahaina Strong</t>
+  </si>
+  <si>
+    <t>$4,853</t>
+  </si>
+  <si>
+    <t>$15,000</t>
+  </si>
+  <si>
+    <t>https://images.gofundme.com/NEfxuaBDIcO2VSFCwS8TAMvQoE4=/720x405/https://d2g8igdw686xgo.cloudfront.net/74679993_1692206848982356_r.jpg</t>
+  </si>
+  <si>
+    <t>The Pratt Family recover from the Lahaina fires</t>
+  </si>
+  <si>
+    <t>$88,504</t>
+  </si>
+  <si>
+    <t>https://images.gofundme.com/TQsNX0YW92XpYC-FAbFpgzCpd9U=/720x405/https://d2g8igdw686xgo.cloudfront.net/74623013_1691620034272980_r.jpeg</t>
+  </si>
+  <si>
+    <t>Help Tomas Family Recover from Lahaina Fires</t>
+  </si>
+  <si>
+    <t>$25,456</t>
+  </si>
+  <si>
+    <t>$30,000</t>
+  </si>
+  <si>
+    <t>https://images.gofundme.com/teziyf0Gd_jOiOKoT0OpniX_-O4=/720x405/https://d2g8igdw686xgo.cloudfront.net/74670847_1691812283590372_r.png</t>
+  </si>
+  <si>
+    <t>The Balisco Family: Lahaina Fire Rebuild Fund</t>
+  </si>
+  <si>
+    <t>$10,951</t>
+  </si>
+  <si>
+    <t>https://images.gofundme.com/o7k1ik4Zpn_CCAA2CZ-zHsC3f_A=/720x405/https://d2g8igdw686xgo.cloudfront.net/74673735_1691802340440917_r.jpeg</t>
+  </si>
+  <si>
+    <t>Valerye &amp; Eric Zimmerman</t>
+  </si>
+  <si>
+    <t>$38,253</t>
+  </si>
+  <si>
+    <t>$45,000</t>
+  </si>
+  <si>
+    <t>https://images.gofundme.com/USj0CrE5waD0A_ZAievLD6Z1HIY=/720x405/https://d2g8igdw686xgo.cloudfront.net/74623655_1691621606899662_r.jpeg</t>
+  </si>
+  <si>
+    <t>The Okano-Kanamu family</t>
+  </si>
+  <si>
+    <t>$26,944</t>
+  </si>
+  <si>
+    <t>https://images.gofundme.com/uFGZzFKuWCo_mFWQwJmZYJWU60A=/720x405/https://d2g8igdw686xgo.cloudfront.net/74621459_1691618585545553_r.jpeg</t>
+  </si>
+  <si>
+    <t>To our uncertain future</t>
+  </si>
+  <si>
+    <t>$19,056</t>
+  </si>
+  <si>
+    <t>https://images.gofundme.com/PUZuSeEZQpXSjLYwVtTQ1onFQoU=/720x405/https://d2g8igdw686xgo.cloudfront.net/74633645_169166247637208_r.jpeg</t>
+  </si>
+  <si>
     <t>The Pasion and Ige Ohana</t>
   </si>
   <si>
@@ -40,127 +148,64 @@
     <t>https://images.gofundme.com/0ys-g3k9KYWOQu3m40hagweQVYA=/720x405/https://d2g8igdw686xgo.cloudfront.net/74680227_1691827777740452_r.jpeg</t>
   </si>
   <si>
+    <t>Lazarte Family: Maui Wildfire Relief</t>
+  </si>
+  <si>
+    <t>$15,839</t>
+  </si>
+  <si>
+    <t>$250,000</t>
+  </si>
+  <si>
+    <t>https://images.gofundme.com/ISXxPMJwpa_vMQIwiosTL-S8dqc=/720x405/https://d2g8igdw686xgo.cloudfront.net/74626245_1691629862463718_r.jpeg</t>
+  </si>
+  <si>
+    <t>The Simbe ‘Ohana GoFundMe</t>
+  </si>
+  <si>
+    <t>$10,541</t>
+  </si>
+  <si>
+    <t>https://images.gofundme.com/CNdbtfSp4tyMIx2aC3DC4bbB3LI=/720x405/https://d2g8igdw686xgo.cloudfront.net/74664295_1691772826725735_r.jpeg</t>
+  </si>
+  <si>
+    <t>UNCLE BULLY AND OHANA</t>
+  </si>
+  <si>
+    <t>$54,992</t>
+  </si>
+  <si>
+    <t>$25,000</t>
+  </si>
+  <si>
+    <t>https://images.gofundme.com/KSx-wOtwaUueYUTEbnomN4M5Xm8=/720x405/https://d2g8igdw686xgo.cloudfront.net/74628965_1691636466155413_r.jpeg</t>
+  </si>
+  <si>
+    <t>Support the Gaastra Family</t>
+  </si>
+  <si>
+    <t>$33,440</t>
+  </si>
+  <si>
+    <t>https://images.gofundme.com/SMyzREhws94XLIKFi6cdlc1EqE0=/720x405/https://d2g8igdw686xgo.cloudfront.net/74641105_1691689560466524_r.jpeg</t>
+  </si>
+  <si>
     <t>Help support the Shultz and Medeiros Families</t>
   </si>
   <si>
     <t>$13,092</t>
   </si>
   <si>
-    <t>$20,000</t>
-  </si>
-  <si>
     <t>https://images.gofundme.com/AM6t97UjV4SnEDqOlVe8sBF2_xE=/720x405/https://d2g8igdw686xgo.cloudfront.net/74687325_1691863234337184_r.jpeg</t>
   </si>
   <si>
-    <t>Valerye &amp; Eric Zimmerman</t>
-  </si>
-  <si>
-    <t>$38,253</t>
-  </si>
-  <si>
-    <t>$45,000</t>
-  </si>
-  <si>
-    <t>https://images.gofundme.com/USj0CrE5waD0A_ZAievLD6Z1HIY=/720x405/https://d2g8igdw686xgo.cloudfront.net/74623655_1691621606899662_r.jpeg</t>
-  </si>
-  <si>
-    <t>Takafua Family Wildfire in Lahaina</t>
-  </si>
-  <si>
-    <t>$8,306</t>
-  </si>
-  <si>
-    <t>$100,000</t>
-  </si>
-  <si>
-    <t>https://images.gofundme.com/53DmfUFhgRdHzs8CJkFdtW0XNnY=/720x405/https://d2g8igdw686xgo.cloudfront.net/74675893_1692732096230158_r.jpg</t>
-  </si>
-  <si>
-    <t>The Balisco Family: Lahaina Fire Rebuild Fund</t>
-  </si>
-  <si>
-    <t>$10,951</t>
-  </si>
-  <si>
-    <t>$15,000</t>
-  </si>
-  <si>
-    <t>https://images.gofundme.com/o7k1ik4Zpn_CCAA2CZ-zHsC3f_A=/720x405/https://d2g8igdw686xgo.cloudfront.net/74673735_1691802340440917_r.jpeg</t>
-  </si>
-  <si>
-    <t>The Casco Ohana affected by the Lahaina Fire</t>
-  </si>
-  <si>
-    <t>$59,060</t>
-  </si>
-  <si>
-    <t>$60,000</t>
-  </si>
-  <si>
-    <t>https://images.gofundme.com/-ni-okGZOFouWUbBuTswBKrJZok=/720x405/https://d2g8igdw686xgo.cloudfront.net/74641605_1691693515709506_r.jpeg</t>
-  </si>
-  <si>
-    <t>Support the Gaastra Family</t>
-  </si>
-  <si>
-    <t>$33,440</t>
-  </si>
-  <si>
-    <t>$25,000</t>
-  </si>
-  <si>
-    <t>https://images.gofundme.com/SMyzREhws94XLIKFi6cdlc1EqE0=/720x405/https://d2g8igdw686xgo.cloudfront.net/74641105_1691689560466524_r.jpeg</t>
-  </si>
-  <si>
-    <t>Lazarte Family: Maui Wildfire Relief</t>
-  </si>
-  <si>
-    <t>$15,839</t>
-  </si>
-  <si>
-    <t>$250,000</t>
-  </si>
-  <si>
-    <t>https://images.gofundme.com/ISXxPMJwpa_vMQIwiosTL-S8dqc=/720x405/https://d2g8igdw686xgo.cloudfront.net/74626245_1691629862463718_r.jpeg</t>
-  </si>
-  <si>
-    <t>The Okano-Kanamu family</t>
-  </si>
-  <si>
-    <t>$26,944</t>
-  </si>
-  <si>
-    <t>$30,000</t>
-  </si>
-  <si>
-    <t>https://images.gofundme.com/uFGZzFKuWCo_mFWQwJmZYJWU60A=/720x405/https://d2g8igdw686xgo.cloudfront.net/74621459_1691618585545553_r.jpeg</t>
-  </si>
-  <si>
-    <t>The Pratt Family recover from the Lahaina fires</t>
-  </si>
-  <si>
-    <t>$88,504</t>
-  </si>
-  <si>
-    <t>https://images.gofundme.com/TQsNX0YW92XpYC-FAbFpgzCpd9U=/720x405/https://d2g8igdw686xgo.cloudfront.net/74623013_1691620034272980_r.jpeg</t>
-  </si>
-  <si>
-    <t>The Simbe ‘Ohana GoFundMe</t>
-  </si>
-  <si>
-    <t>$10,541</t>
-  </si>
-  <si>
-    <t>https://images.gofundme.com/CNdbtfSp4tyMIx2aC3DC4bbB3LI=/720x405/https://d2g8igdw686xgo.cloudfront.net/74664295_1691772826725735_r.jpeg</t>
-  </si>
-  <si>
-    <t>Timko Family Lahaina Wildfire Relief Fund</t>
-  </si>
-  <si>
-    <t>$12,540</t>
-  </si>
-  <si>
-    <t>https://images.gofundme.com/c1UhbqWgLfq7yZCWg4xtWuIIGio=/720x405/https://d2g8igdw686xgo.cloudfront.net/74647267_1691705408863508_r.jpeg</t>
+    <t>Tommy Kealoha Lahaina Fire</t>
+  </si>
+  <si>
+    <t>$15,908</t>
+  </si>
+  <si>
+    <t>https://images.gofundme.com/qZcIc5LWPHZ2pBqPzd66ntodayQ=/720x405/https://d2g8igdw686xgo.cloudfront.net/74623371_1691621264948677_r.jpeg</t>
   </si>
   <si>
     <t>To our kids future-Lahaina</t>
@@ -173,51 +218,6 @@
   </si>
   <si>
     <t>https://images.gofundme.com/suqkSNaiOt1yUqcFE0Zo66C7VAY=/720x405/https://d2g8igdw686xgo.cloudfront.net/74661783_169176524697822_r.jpeg</t>
-  </si>
-  <si>
-    <t>To our uncertain future</t>
-  </si>
-  <si>
-    <t>$19,056</t>
-  </si>
-  <si>
-    <t>https://images.gofundme.com/PUZuSeEZQpXSjLYwVtTQ1onFQoU=/720x405/https://d2g8igdw686xgo.cloudfront.net/74633645_169166247637208_r.jpeg</t>
-  </si>
-  <si>
-    <t>Help Tomas Family Recover from Lahaina Fires</t>
-  </si>
-  <si>
-    <t>$25,456</t>
-  </si>
-  <si>
-    <t>https://images.gofundme.com/teziyf0Gd_jOiOKoT0OpniX_-O4=/720x405/https://d2g8igdw686xgo.cloudfront.net/74670847_1691812283590372_r.png</t>
-  </si>
-  <si>
-    <t>Tommy Kealoha Lahaina Fire</t>
-  </si>
-  <si>
-    <t>$15,908</t>
-  </si>
-  <si>
-    <t>https://images.gofundme.com/qZcIc5LWPHZ2pBqPzd66ntodayQ=/720x405/https://d2g8igdw686xgo.cloudfront.net/74623371_1691621264948677_r.jpeg</t>
-  </si>
-  <si>
-    <t>Lahaina Strong</t>
-  </si>
-  <si>
-    <t>$4,853</t>
-  </si>
-  <si>
-    <t>https://images.gofundme.com/NEfxuaBDIcO2VSFCwS8TAMvQoE4=/720x405/https://d2g8igdw686xgo.cloudfront.net/74679993_1692206848982356_r.jpg</t>
-  </si>
-  <si>
-    <t>UNCLE BULLY AND OHANA</t>
-  </si>
-  <si>
-    <t>$54,992</t>
-  </si>
-  <si>
-    <t>https://images.gofundme.com/KSx-wOtwaUueYUTEbnomN4M5Xm8=/720x405/https://d2g8igdw686xgo.cloudfront.net/74628965_1691636466155413_r.jpeg</t>
   </si>
   <si>
     <t>Urgent Help for Jennifer Yi after Maui Wildfire</t>
@@ -687,80 +687,80 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
         <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
         <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -771,119 +771,119 @@
         <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
         <v>54</v>
       </c>
-      <c r="B16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" t="s">
         <v>66</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>67</v>
-      </c>
-      <c r="C20" t="s">
-        <v>31</v>
       </c>
       <c r="D20" t="s">
         <v>68</v>
@@ -897,7 +897,7 @@
         <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
         <v>71</v>

</xml_diff>